<commit_message>
add something to start分析
</commit_message>
<xml_diff>
--- a/linux-2.6.32.27_compressed.xlsx
+++ b/linux-2.6.32.27_compressed.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="2"/>
@@ -10,15 +10,16 @@
     <sheet name="表纸" sheetId="4" r:id="rId1"/>
     <sheet name="目录" sheetId="5" r:id="rId2"/>
     <sheet name="start分析" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="cache_on分析" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="resource" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="100">
   <si>
     <t>结束日期：</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -321,12 +322,163 @@
     <t>0地址处执行则需要运行下面的重定位处理，否则跳转到not_relocated处执行。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>（1）对bss节清零</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r2中存放的是bss的起始地址，r3总存放的是bss节的结束地址，上面代码对bss进行清零。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（2）cache_on处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（3）备份sp的值到r1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（4）r2 = sp + 64K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>执行完上面操作后，寄存器中存放的值如下所示：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存放的是LC0符号的链接地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存放的是 _image_size = (_etext - _text) * 4;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_got_start</t>
+  </si>
+  <si>
+    <t>ip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_got_end</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reloc_end:vmlinux代码段的结束，后面就是堆栈段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reloc_start:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cache_on分析</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>在C语言运行环境准备好之前会执行cache_on函数，用于打开CPU cache功能。打开cache功能之前需要先设置页表（需要使用D-Cache）,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存放的是LC0符号的运行时地址与LC0链接地址的差值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存放的是__bss_start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存放的是_end，即bss段的结束地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存放的是zreladdr，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于zreladdr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zreladdr在 arch/arm/boot/compressed/Makefile 中定义：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LDFLAGS_vmlinux := --defsym </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>zreladdr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=$(ZRELADDR)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZRELADDR在 arch/arm/boot/Makefile 中定义，并进行了export</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zreladdr-y 在 arch/arm/mach-s3c2410/Makefile.boot:1:   zreladdr-y     := 0x30008000 中定义。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,6 +548,21 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -567,7 +734,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -590,20 +757,20 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -627,20 +794,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -649,6 +817,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -792,194 +968,6 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="矩形标注 5"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10134600" y="2609850"/>
-          <a:ext cx="1362075" cy="762000"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -204387"/>
-            <a:gd name="adj2" fmla="val -4167"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="15875">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>程序应该从</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>_start</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>符号开始执行</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="矩形标注 7"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12030075" y="7972425"/>
-          <a:ext cx="1362075" cy="762000"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -204387"/>
-            <a:gd name="adj2" fmla="val -4167"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="15875">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>程序应该从</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>_start</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>符号开始执行</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -1135,128 +1123,6 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="TextBox 10"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11658600" y="10372725"/>
-          <a:ext cx="361949" cy="323850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>①</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="矩形 11"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13030200" y="10010775"/>
-          <a:ext cx="1647825" cy="504825"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="15875">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -1718,13 +1584,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>213</xdr:row>
+      <xdr:row>236</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>256</xdr:row>
+      <xdr:row>279</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1759,6 +1625,500 @@
         <a:effectLst/>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>283</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>103819</xdr:colOff>
+      <xdr:row>298</xdr:row>
+      <xdr:rowOff>142518</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="47110650"/>
+          <a:ext cx="7647619" cy="2857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>283</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>289</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="矩形 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2590800" y="47272575"/>
+          <a:ext cx="2047875" cy="1000125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>332733</xdr:colOff>
+      <xdr:row>217</xdr:row>
+      <xdr:rowOff>142835</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7543800" y="39147750"/>
+          <a:ext cx="5133333" cy="323810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>618276</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>132905</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="514350"/>
+          <a:ext cx="6790476" cy="3561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="矩形标注 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4495800" y="1171575"/>
+          <a:ext cx="1362075" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -204387"/>
+            <a:gd name="adj2" fmla="val -4167"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>程序应该从</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>_start</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>符号开始执行</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形标注 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3800475" y="5553075"/>
+          <a:ext cx="1362075" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -204387"/>
+            <a:gd name="adj2" fmla="val -4167"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>程序应该从</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>_start</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>符号开始执行</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="7934325"/>
+          <a:ext cx="361949" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>①</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="矩形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4800600" y="7572375"/>
+          <a:ext cx="1647825" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2074,12 +2434,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:M39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="3" width="9" style="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
@@ -2087,71 +2447,71 @@
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:13" ht="15" thickBot="1"/>
-    <row r="4" spans="4:13" ht="15" thickTop="1">
-      <c r="D4" s="19" t="s">
+    <row r="3" spans="4:13" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="4:13" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="D4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="21"/>
-    </row>
-    <row r="5" spans="4:13">
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
-    </row>
-    <row r="6" spans="4:13">
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="24"/>
-    </row>
-    <row r="7" spans="4:13">
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="24"/>
-    </row>
-    <row r="8" spans="4:13" ht="15" thickBot="1">
-      <c r="D8" s="25"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="27"/>
-    </row>
-    <row r="9" spans="4:13" ht="15" thickTop="1"/>
-    <row r="12" spans="4:13">
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="19"/>
+    </row>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="D5" s="20"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="22"/>
+    </row>
+    <row r="6" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="22"/>
+    </row>
+    <row r="7" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="22"/>
+    </row>
+    <row r="8" spans="4:13" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="25"/>
+    </row>
+    <row r="9" spans="4:13" ht="15" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
@@ -2159,7 +2519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="4:13">
+    <row r="14" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2167,12 +2527,12 @@
         <v>42700</v>
       </c>
     </row>
-    <row r="16" spans="4:13">
+    <row r="16" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:13">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2180,197 +2540,221 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="4:13">
-      <c r="G22" s="28" t="s">
+    <row r="22" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="G22" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="29"/>
-      <c r="I22" s="28" t="s">
+      <c r="H22" s="16"/>
+      <c r="I22" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="29"/>
-    </row>
-    <row r="23" spans="4:13">
-      <c r="G23" s="28" t="s">
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="G23" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H23" s="29"/>
-      <c r="I23" s="28" t="s">
+      <c r="H23" s="16"/>
+      <c r="I23" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J23" s="29"/>
-    </row>
-    <row r="24" spans="4:13">
-      <c r="G24" s="28" t="s">
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="G24" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="29"/>
-      <c r="I24" s="28" t="s">
+      <c r="H24" s="16"/>
+      <c r="I24" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="29"/>
-    </row>
-    <row r="27" spans="4:13">
+      <c r="J24" s="16"/>
+    </row>
+    <row r="27" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D27" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="4:13">
+    <row r="28" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="12" t="s">
+      <c r="F28" s="27"/>
+      <c r="G28" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="13"/>
-    </row>
-    <row r="29" spans="4:13">
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="27"/>
+    </row>
+    <row r="29" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="29">
         <v>42700</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="16"/>
-    </row>
-    <row r="30" spans="4:13">
+      <c r="F29" s="27"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="32"/>
+    </row>
+    <row r="30" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D30" s="4"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="16"/>
-    </row>
-    <row r="31" spans="4:13">
+      <c r="E30" s="29"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="32"/>
+    </row>
+    <row r="31" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D31" s="3"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="16"/>
-    </row>
-    <row r="32" spans="4:13">
+      <c r="E31" s="26"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="32"/>
+    </row>
+    <row r="32" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D32" s="3"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="16"/>
-    </row>
-    <row r="33" spans="4:13">
+      <c r="E32" s="26"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="32"/>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D33" s="3"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="16"/>
-    </row>
-    <row r="34" spans="4:13">
+      <c r="E33" s="26"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="32"/>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D34" s="3"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="16"/>
-    </row>
-    <row r="35" spans="4:13">
+      <c r="E34" s="26"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="32"/>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D35" s="3"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="16"/>
-    </row>
-    <row r="36" spans="4:13">
+      <c r="E35" s="26"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="32"/>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D36" s="3"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="16"/>
-    </row>
-    <row r="37" spans="4:13">
+      <c r="E36" s="26"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="32"/>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D37" s="3"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="16"/>
-    </row>
-    <row r="38" spans="4:13">
+      <c r="E37" s="26"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="32"/>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D38" s="3"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="16"/>
-    </row>
-    <row r="39" spans="4:13">
+      <c r="E38" s="26"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="32"/>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.15">
       <c r="D39" s="3"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="16"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:M37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:M38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:M39"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:M34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:M35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:M36"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:M31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:M32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:M33"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:M28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:M29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:M30"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="D4:M8"/>
@@ -2378,30 +2762,6 @@
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="I23:J23"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:M28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:M29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:M30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:M31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:M32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:M33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:M34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:M35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:M36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:M37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:M38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:M39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2410,40 +2770,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="18.75">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C6" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C10" s="7" t="s">
         <v>21</v>
       </c>
@@ -2462,16 +2822,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O610"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O634"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="C258" sqref="C258"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="L220" sqref="L220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" ht="18.75">
+    <row r="1" spans="1:15" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>24</v>
       </c>
@@ -2479,784 +2839,915 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="3" spans="1:15" s="30" customFormat="1" ht="14.25">
-      <c r="B3" s="30" t="s">
+    <row r="2" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B3" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="30" customFormat="1" ht="14.25">
-      <c r="B4" s="30" t="s">
+    <row r="4" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B4" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="30" customFormat="1" ht="14.25">
-      <c r="B5" s="30" t="s">
+    <row r="5" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B5" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="7" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="8" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="9" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="10" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="11" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="12" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="13" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="14" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="15" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="16" spans="1:15" s="30" customFormat="1" ht="14.25"/>
-    <row r="17" s="30" customFormat="1" ht="14.25"/>
-    <row r="18" s="30" customFormat="1" ht="14.25"/>
-    <row r="19" s="30" customFormat="1" ht="14.25"/>
-    <row r="20" s="30" customFormat="1" ht="14.25"/>
-    <row r="21" s="30" customFormat="1" ht="14.25"/>
-    <row r="22" s="30" customFormat="1" ht="14.25"/>
-    <row r="23" s="30" customFormat="1" ht="14.25"/>
-    <row r="24" s="30" customFormat="1" ht="14.25"/>
-    <row r="25" s="30" customFormat="1" ht="14.25"/>
-    <row r="26" s="30" customFormat="1" ht="14.25"/>
-    <row r="27" s="30" customFormat="1" ht="14.25"/>
-    <row r="28" s="30" customFormat="1" ht="14.25"/>
-    <row r="29" s="30" customFormat="1" ht="14.25"/>
-    <row r="30" s="30" customFormat="1" ht="14.25"/>
-    <row r="31" s="30" customFormat="1" ht="14.25"/>
-    <row r="32" s="30" customFormat="1" ht="14.25"/>
-    <row r="33" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="34" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="35" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="36" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="37" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="38" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="39" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="40" spans="2:2" s="30" customFormat="1" ht="14.25">
-      <c r="B40" s="30" t="s">
+    <row r="6" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:15" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="17" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="18" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="19" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="20" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="21" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="22" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="23" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="24" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="25" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="26" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="27" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="28" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="29" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="30" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="31" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="32" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="33" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="34" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="35" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="36" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="37" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="38" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="39" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="40" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B40" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:2" s="30" customFormat="1" ht="14.25">
-      <c r="B41" s="30" t="s">
+    <row r="41" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B41" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="43" spans="2:2" s="30" customFormat="1" ht="14.25">
-      <c r="B43" s="30" t="s">
+    <row r="42" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="43" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B43" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="45" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="46" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="47" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="48" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="49" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="50" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="51" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="52" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="53" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="54" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="55" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="56" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="57" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="58" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="59" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="60" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="61" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="62" spans="2:5" s="30" customFormat="1" ht="14.25"/>
-    <row r="63" spans="2:5" s="30" customFormat="1" ht="14.25">
-      <c r="B63" s="30" t="s">
+    <row r="44" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="45" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="46" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="47" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="49" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="50" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="51" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="52" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="53" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="54" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="55" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="56" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="57" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="58" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="59" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="60" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="61" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="62" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="63" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B63" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="2:5" s="30" customFormat="1" ht="14.25">
-      <c r="C64" s="30" t="s">
+    <row r="64" spans="2:5" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C64" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E64" s="30" t="s">
+      <c r="E64" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="2:11" s="30" customFormat="1" ht="14.25">
-      <c r="C65" s="30" t="s">
+    <row r="65" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C65" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E65" s="30" t="s">
+      <c r="E65" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="2:11" s="30" customFormat="1" ht="14.25"/>
-    <row r="67" spans="2:11" s="30" customFormat="1" ht="14.25">
-      <c r="C67" s="30" t="s">
+    <row r="66" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="67" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C67" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="2:11" s="30" customFormat="1" ht="14.25">
-      <c r="D68" s="32" t="s">
+    <row r="68" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="D68" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="2:11" s="30" customFormat="1" ht="14.25"/>
-    <row r="70" spans="2:11" s="30" customFormat="1" ht="14.25">
-      <c r="B70" s="30" t="s">
+    <row r="69" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="70" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B70" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="K70" s="31"/>
-    </row>
-    <row r="71" spans="2:11" s="30" customFormat="1" ht="14.25">
-      <c r="C71" s="30" t="s">
+      <c r="K70" s="13"/>
+    </row>
+    <row r="71" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C71" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F71" s="30" t="s">
+      <c r="F71" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="2:11" s="30" customFormat="1" ht="14.25"/>
-    <row r="73" spans="2:11" s="30" customFormat="1" ht="14.25">
-      <c r="B73" s="30" t="s">
+    <row r="72" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="73" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B73" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="2:11" s="30" customFormat="1" ht="14.25">
-      <c r="C74" s="30" t="s">
+    <row r="74" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C74" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="2:11" s="30" customFormat="1" ht="14.25"/>
-    <row r="76" spans="2:11" s="30" customFormat="1" ht="14.25">
-      <c r="B76" s="30" t="s">
+    <row r="75" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="76" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B76" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="77" spans="2:11" s="30" customFormat="1" ht="14.25"/>
-    <row r="78" spans="2:11" s="30" customFormat="1" ht="14.25">
-      <c r="B78" s="30" t="s">
+    <row r="77" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="78" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B78" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="2:11" s="30" customFormat="1" ht="14.25"/>
-    <row r="80" spans="2:11" s="30" customFormat="1" ht="14.25">
-      <c r="B80" s="30" t="s">
+    <row r="79" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="80" spans="2:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B80" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="2:2" s="30" customFormat="1" ht="14.25">
-      <c r="B81" s="30" t="s">
+    <row r="81" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B81" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="83" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="84" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="85" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="86" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="87" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="88" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="89" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="90" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="91" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="92" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="93" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="94" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="95" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="96" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="97" s="30" customFormat="1" ht="14.25"/>
-    <row r="98" s="30" customFormat="1" ht="14.25"/>
-    <row r="99" s="30" customFormat="1" ht="14.25"/>
-    <row r="100" s="30" customFormat="1" ht="14.25"/>
-    <row r="101" s="30" customFormat="1" ht="14.25"/>
-    <row r="102" s="30" customFormat="1" ht="14.25"/>
-    <row r="103" s="30" customFormat="1" ht="14.25"/>
-    <row r="104" s="30" customFormat="1" ht="14.25"/>
-    <row r="105" s="30" customFormat="1" ht="14.25"/>
-    <row r="106" s="30" customFormat="1" ht="14.25"/>
-    <row r="107" s="30" customFormat="1" ht="14.25"/>
-    <row r="108" s="30" customFormat="1" ht="14.25"/>
-    <row r="109" s="30" customFormat="1" ht="14.25"/>
-    <row r="110" s="30" customFormat="1" ht="14.25"/>
-    <row r="111" s="30" customFormat="1" ht="14.25"/>
-    <row r="112" s="30" customFormat="1" ht="14.25"/>
-    <row r="113" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="114" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="115" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="116" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="117" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="118" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="119" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="120" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="121" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="122" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="123" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="124" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="125" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="126" spans="2:2" s="30" customFormat="1" ht="14.25">
-      <c r="B126" s="30" t="s">
+    <row r="82" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="83" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="84" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="85" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="86" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="87" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="88" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="89" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="90" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="91" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="92" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="93" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="94" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="95" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="96" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="97" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="98" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="99" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="100" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="101" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="102" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="103" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="104" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="105" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="106" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="107" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="108" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="109" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="110" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="111" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="112" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="113" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="114" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="115" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="116" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="117" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="118" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="119" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="120" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="121" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="122" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="123" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="124" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="125" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="126" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B126" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="127" spans="2:2" s="30" customFormat="1" ht="14.25">
-      <c r="B127" s="30" t="s">
+    <row r="127" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B127" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="128" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="129" spans="2:3" s="30" customFormat="1" ht="14.25">
-      <c r="B129" s="30" t="s">
+    <row r="128" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="129" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B129" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="2:3" s="30" customFormat="1" ht="14.25">
-      <c r="B130" s="30" t="s">
+    <row r="130" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B130" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="131" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="132" spans="2:3" s="30" customFormat="1" ht="14.25">
-      <c r="B132" s="30" t="s">
+    <row r="131" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="132" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B132" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C132" s="30" t="s">
+      <c r="C132" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="133" spans="2:3" s="30" customFormat="1" ht="14.25">
-      <c r="C133" s="30" t="s">
+    <row r="133" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C133" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="134" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="135" spans="2:3" s="30" customFormat="1" ht="14.25">
-      <c r="C135" s="30" t="s">
+    <row r="134" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="135" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C135" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="136" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="137" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="138" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="139" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="140" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="141" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="142" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="143" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="144" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="145" s="30" customFormat="1" ht="14.25"/>
-    <row r="146" s="30" customFormat="1" ht="14.25"/>
-    <row r="147" s="30" customFormat="1" ht="14.25"/>
-    <row r="148" s="30" customFormat="1" ht="14.25"/>
-    <row r="149" s="30" customFormat="1" ht="14.25"/>
-    <row r="150" s="30" customFormat="1" ht="14.25"/>
-    <row r="151" s="30" customFormat="1" ht="14.25"/>
-    <row r="152" s="30" customFormat="1" ht="14.25"/>
-    <row r="153" s="30" customFormat="1" ht="14.25"/>
-    <row r="154" s="30" customFormat="1" ht="14.25"/>
-    <row r="155" s="30" customFormat="1" ht="14.25"/>
-    <row r="156" s="30" customFormat="1" ht="14.25"/>
-    <row r="157" s="30" customFormat="1" ht="14.25"/>
-    <row r="158" s="30" customFormat="1" ht="14.25"/>
-    <row r="159" s="30" customFormat="1" ht="14.25"/>
-    <row r="160" s="30" customFormat="1" ht="14.25"/>
-    <row r="161" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="162" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="163" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="164" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="165" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="166" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="167" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="168" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="169" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="170" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="171" spans="2:2" s="30" customFormat="1" ht="14.25">
-      <c r="B171" s="30" t="s">
+    <row r="136" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="137" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="138" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="139" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="140" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="141" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="142" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="143" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="144" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="145" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="146" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="147" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="148" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="149" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="150" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="151" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="152" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="153" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="154" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="155" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="156" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="157" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="158" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="159" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="160" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="161" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="162" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="163" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="164" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="165" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="166" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="167" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="168" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="169" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="170" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="171" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B171" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="172" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="173" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="174" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="175" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="176" spans="2:2" s="30" customFormat="1" ht="14.25"/>
-    <row r="177" spans="2:4" s="30" customFormat="1" ht="14.25"/>
-    <row r="178" spans="2:4" s="30" customFormat="1" ht="14.25"/>
-    <row r="179" spans="2:4" s="30" customFormat="1" ht="14.25"/>
-    <row r="180" spans="2:4" s="30" customFormat="1" ht="14.25"/>
-    <row r="181" spans="2:4" s="30" customFormat="1" ht="14.25"/>
-    <row r="182" spans="2:4" s="30" customFormat="1" ht="14.25"/>
-    <row r="183" spans="2:4" s="30" customFormat="1" ht="14.25">
-      <c r="B183" s="30" t="s">
+    <row r="172" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="173" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="174" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="175" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="176" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="177" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="178" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="179" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="180" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="181" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="182" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="183" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B183" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="184" spans="2:4" s="30" customFormat="1" ht="14.25">
-      <c r="C184" s="30" t="s">
+    <row r="184" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C184" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="185" spans="2:4" s="30" customFormat="1" ht="14.25"/>
-    <row r="186" spans="2:4" s="30" customFormat="1" ht="14.25">
-      <c r="C186" s="30" t="s">
+    <row r="185" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="186" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C186" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="187" spans="2:4" s="30" customFormat="1" ht="14.25">
-      <c r="D187" s="30" t="s">
+    <row r="187" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="D187" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="188" spans="2:4" s="30" customFormat="1" ht="14.25"/>
-    <row r="189" spans="2:4" s="30" customFormat="1" ht="14.25">
-      <c r="B189" s="30" t="s">
+    <row r="188" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="189" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B189" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="190" spans="2:4" s="30" customFormat="1" ht="14.25">
-      <c r="C190" s="30" t="s">
+    <row r="190" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C190" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="191" spans="2:4" s="30" customFormat="1" ht="14.25">
-      <c r="C191" s="30" t="s">
+    <row r="191" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C191" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="192" spans="2:4" s="30" customFormat="1" ht="14.25"/>
-    <row r="193" spans="2:3" s="30" customFormat="1" ht="14.25">
-      <c r="C193" s="30" t="s">
+    <row r="192" spans="2:4" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="193" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C193" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="194" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="195" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="196" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="197" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="198" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="199" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="200" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="201" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="202" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="203" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="204" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="205" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="206" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="207" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="208" spans="2:3" s="30" customFormat="1" ht="14.25">
-      <c r="B208" s="30" t="s">
+    <row r="194" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="195" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="196" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="197" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="198" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="199" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="200" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="201" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="202" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="203" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="204" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="205" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="206" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="207" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="208" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B208" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="209" spans="2:3" s="30" customFormat="1" ht="14.25">
-      <c r="C209" s="30" t="s">
+    <row r="209" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C209" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="210" spans="2:3" s="30" customFormat="1" ht="14.25">
-      <c r="C210" s="30" t="s">
+    <row r="210" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C210" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="211" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="212" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="213" spans="2:3" s="30" customFormat="1" ht="14.25">
-      <c r="B213" s="30" t="s">
+    <row r="211" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="212" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="213" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B213" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L213" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="214" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C214" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D214" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="L214" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="215" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C215" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D215" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="L215" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="216" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C216" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D216" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="L216" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="217" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C217" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D217" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="218" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C218" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D218" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="219" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C219" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D219" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="L219" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="220" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C220" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D220" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="221" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C221" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D221" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="222" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C222" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="223" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="224" spans="2:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C224" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="225" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C225" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="226" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="227" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="228" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="229" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="230" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="231" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="232" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="233" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="234" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="235" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="236" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B236" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="214" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="215" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="216" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="217" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="218" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="219" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="220" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="221" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="222" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="223" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="224" spans="2:3" s="30" customFormat="1" ht="14.25"/>
-    <row r="225" s="30" customFormat="1" ht="14.25"/>
-    <row r="226" s="30" customFormat="1" ht="14.25"/>
-    <row r="227" s="30" customFormat="1" ht="14.25"/>
-    <row r="228" s="30" customFormat="1" ht="14.25"/>
-    <row r="229" s="30" customFormat="1" ht="14.25"/>
-    <row r="230" s="30" customFormat="1" ht="14.25"/>
-    <row r="231" s="30" customFormat="1" ht="14.25"/>
-    <row r="232" s="30" customFormat="1" ht="14.25"/>
-    <row r="233" s="30" customFormat="1" ht="14.25"/>
-    <row r="234" s="30" customFormat="1" ht="14.25"/>
-    <row r="235" s="30" customFormat="1" ht="14.25"/>
-    <row r="236" s="30" customFormat="1" ht="14.25"/>
-    <row r="237" s="30" customFormat="1" ht="14.25"/>
-    <row r="238" s="30" customFormat="1" ht="14.25"/>
-    <row r="239" s="30" customFormat="1" ht="14.25"/>
-    <row r="240" s="30" customFormat="1" ht="14.25"/>
-    <row r="241" s="30" customFormat="1" ht="14.25"/>
-    <row r="242" s="30" customFormat="1" ht="14.25"/>
-    <row r="243" s="30" customFormat="1" ht="14.25"/>
-    <row r="244" s="30" customFormat="1" ht="14.25"/>
-    <row r="245" s="30" customFormat="1" ht="14.25"/>
-    <row r="246" s="30" customFormat="1" ht="14.25"/>
-    <row r="247" s="30" customFormat="1" ht="14.25"/>
-    <row r="248" s="30" customFormat="1" ht="14.25"/>
-    <row r="249" s="30" customFormat="1" ht="14.25"/>
-    <row r="250" s="30" customFormat="1" ht="14.25"/>
-    <row r="251" s="30" customFormat="1" ht="14.25"/>
-    <row r="252" s="30" customFormat="1" ht="14.25"/>
-    <row r="253" s="30" customFormat="1" ht="14.25"/>
-    <row r="254" s="30" customFormat="1" ht="14.25"/>
-    <row r="255" s="30" customFormat="1" ht="14.25"/>
-    <row r="256" s="30" customFormat="1" ht="14.25"/>
-    <row r="257" s="30" customFormat="1" ht="14.25"/>
-    <row r="258" s="30" customFormat="1" ht="14.25"/>
-    <row r="259" s="30" customFormat="1" ht="14.25"/>
-    <row r="260" s="30" customFormat="1" ht="14.25"/>
-    <row r="261" s="30" customFormat="1" ht="14.25"/>
-    <row r="262" s="30" customFormat="1" ht="14.25"/>
-    <row r="263" s="30" customFormat="1" ht="14.25"/>
-    <row r="264" s="30" customFormat="1" ht="14.25"/>
-    <row r="265" s="30" customFormat="1" ht="14.25"/>
-    <row r="266" s="30" customFormat="1" ht="14.25"/>
-    <row r="267" s="30" customFormat="1" ht="14.25"/>
-    <row r="268" s="30" customFormat="1" ht="14.25"/>
-    <row r="269" s="30" customFormat="1" ht="14.25"/>
-    <row r="270" s="30" customFormat="1" ht="14.25"/>
-    <row r="271" s="30" customFormat="1" ht="14.25"/>
-    <row r="272" s="30" customFormat="1" ht="14.25"/>
-    <row r="273" s="30" customFormat="1" ht="14.25"/>
-    <row r="274" s="30" customFormat="1" ht="14.25"/>
-    <row r="275" s="30" customFormat="1" ht="14.25"/>
-    <row r="276" s="30" customFormat="1" ht="14.25"/>
-    <row r="277" s="30" customFormat="1" ht="14.25"/>
-    <row r="278" s="30" customFormat="1" ht="14.25"/>
-    <row r="279" s="30" customFormat="1" ht="14.25"/>
-    <row r="280" s="30" customFormat="1" ht="14.25"/>
-    <row r="281" s="30" customFormat="1" ht="14.25"/>
-    <row r="282" s="30" customFormat="1" ht="14.25"/>
-    <row r="283" s="30" customFormat="1" ht="14.25"/>
-    <row r="284" s="30" customFormat="1" ht="14.25"/>
-    <row r="285" s="30" customFormat="1" ht="14.25"/>
-    <row r="286" s="30" customFormat="1" ht="14.25"/>
-    <row r="287" s="30" customFormat="1" ht="14.25"/>
-    <row r="288" s="30" customFormat="1" ht="14.25"/>
-    <row r="289" s="30" customFormat="1" ht="14.25"/>
-    <row r="290" s="30" customFormat="1" ht="14.25"/>
-    <row r="291" s="30" customFormat="1" ht="14.25"/>
-    <row r="292" s="30" customFormat="1" ht="14.25"/>
-    <row r="293" s="30" customFormat="1" ht="14.25"/>
-    <row r="294" s="30" customFormat="1" ht="14.25"/>
-    <row r="295" s="30" customFormat="1" ht="14.25"/>
-    <row r="296" s="30" customFormat="1" ht="14.25"/>
-    <row r="297" s="30" customFormat="1" ht="14.25"/>
-    <row r="298" s="30" customFormat="1" ht="14.25"/>
-    <row r="299" s="30" customFormat="1" ht="14.25"/>
-    <row r="300" s="30" customFormat="1" ht="14.25"/>
-    <row r="301" s="30" customFormat="1" ht="14.25"/>
-    <row r="302" s="30" customFormat="1" ht="14.25"/>
-    <row r="303" s="30" customFormat="1" ht="14.25"/>
-    <row r="304" s="30" customFormat="1" ht="14.25"/>
-    <row r="305" s="30" customFormat="1" ht="14.25"/>
-    <row r="306" s="30" customFormat="1" ht="14.25"/>
-    <row r="307" s="30" customFormat="1" ht="14.25"/>
-    <row r="308" s="30" customFormat="1" ht="14.25"/>
-    <row r="309" s="30" customFormat="1" ht="14.25"/>
-    <row r="310" s="30" customFormat="1" ht="14.25"/>
-    <row r="311" s="30" customFormat="1" ht="14.25"/>
-    <row r="312" s="30" customFormat="1" ht="14.25"/>
-    <row r="313" s="30" customFormat="1" ht="14.25"/>
-    <row r="314" s="30" customFormat="1" ht="14.25"/>
-    <row r="315" s="30" customFormat="1" ht="14.25"/>
-    <row r="316" s="30" customFormat="1" ht="14.25"/>
-    <row r="317" s="30" customFormat="1" ht="14.25"/>
-    <row r="318" s="30" customFormat="1" ht="14.25"/>
-    <row r="319" s="30" customFormat="1" ht="14.25"/>
-    <row r="320" s="30" customFormat="1" ht="14.25"/>
-    <row r="321" s="30" customFormat="1" ht="14.25"/>
-    <row r="322" s="30" customFormat="1" ht="14.25"/>
-    <row r="323" s="30" customFormat="1" ht="14.25"/>
-    <row r="324" s="30" customFormat="1" ht="14.25"/>
-    <row r="325" s="30" customFormat="1" ht="14.25"/>
-    <row r="326" s="30" customFormat="1" ht="14.25"/>
-    <row r="327" s="30" customFormat="1" ht="14.25"/>
-    <row r="328" s="30" customFormat="1" ht="14.25"/>
-    <row r="329" s="30" customFormat="1" ht="14.25"/>
-    <row r="330" s="30" customFormat="1" ht="14.25"/>
-    <row r="331" s="30" customFormat="1" ht="14.25"/>
-    <row r="332" s="30" customFormat="1" ht="14.25"/>
-    <row r="333" s="30" customFormat="1" ht="14.25"/>
-    <row r="334" s="30" customFormat="1" ht="14.25"/>
-    <row r="335" s="30" customFormat="1" ht="14.25"/>
-    <row r="336" s="30" customFormat="1" ht="14.25"/>
-    <row r="337" s="30" customFormat="1" ht="14.25"/>
-    <row r="338" s="30" customFormat="1" ht="14.25"/>
-    <row r="339" s="30" customFormat="1" ht="14.25"/>
-    <row r="340" s="30" customFormat="1" ht="14.25"/>
-    <row r="341" s="30" customFormat="1" ht="14.25"/>
-    <row r="342" s="30" customFormat="1" ht="14.25"/>
-    <row r="343" s="30" customFormat="1" ht="14.25"/>
-    <row r="344" s="30" customFormat="1" ht="14.25"/>
-    <row r="345" s="30" customFormat="1" ht="14.25"/>
-    <row r="346" s="30" customFormat="1" ht="14.25"/>
-    <row r="347" s="30" customFormat="1" ht="14.25"/>
-    <row r="348" s="30" customFormat="1" ht="14.25"/>
-    <row r="349" s="30" customFormat="1" ht="14.25"/>
-    <row r="350" s="30" customFormat="1" ht="14.25"/>
-    <row r="351" s="30" customFormat="1" ht="14.25"/>
-    <row r="352" s="30" customFormat="1" ht="14.25"/>
-    <row r="353" s="30" customFormat="1" ht="14.25"/>
-    <row r="354" s="30" customFormat="1" ht="14.25"/>
-    <row r="355" s="30" customFormat="1" ht="14.25"/>
-    <row r="356" s="30" customFormat="1" ht="14.25"/>
-    <row r="357" s="30" customFormat="1" ht="14.25"/>
-    <row r="358" s="30" customFormat="1" ht="14.25"/>
-    <row r="359" s="30" customFormat="1" ht="14.25"/>
-    <row r="360" s="30" customFormat="1" ht="14.25"/>
-    <row r="361" s="30" customFormat="1" ht="14.25"/>
-    <row r="362" s="30" customFormat="1" ht="14.25"/>
-    <row r="363" s="30" customFormat="1" ht="14.25"/>
-    <row r="364" s="30" customFormat="1" ht="14.25"/>
-    <row r="365" s="30" customFormat="1" ht="14.25"/>
-    <row r="366" s="30" customFormat="1" ht="14.25"/>
-    <row r="367" s="30" customFormat="1" ht="14.25"/>
-    <row r="368" s="30" customFormat="1" ht="14.25"/>
-    <row r="369" s="30" customFormat="1" ht="14.25"/>
-    <row r="370" s="30" customFormat="1" ht="14.25"/>
-    <row r="371" s="30" customFormat="1" ht="14.25"/>
-    <row r="372" s="30" customFormat="1" ht="14.25"/>
-    <row r="373" s="30" customFormat="1" ht="14.25"/>
-    <row r="374" s="30" customFormat="1" ht="14.25"/>
-    <row r="375" s="30" customFormat="1" ht="14.25"/>
-    <row r="376" s="30" customFormat="1" ht="14.25"/>
-    <row r="377" s="30" customFormat="1" ht="14.25"/>
-    <row r="378" s="30" customFormat="1" ht="14.25"/>
-    <row r="379" s="30" customFormat="1" ht="14.25"/>
-    <row r="380" s="30" customFormat="1" ht="14.25"/>
-    <row r="381" s="30" customFormat="1" ht="14.25"/>
-    <row r="382" s="30" customFormat="1" ht="14.25"/>
-    <row r="383" s="30" customFormat="1" ht="14.25"/>
-    <row r="384" s="30" customFormat="1" ht="14.25"/>
-    <row r="385" s="30" customFormat="1" ht="14.25"/>
-    <row r="386" s="30" customFormat="1" ht="14.25"/>
-    <row r="387" s="30" customFormat="1" ht="14.25"/>
-    <row r="388" s="30" customFormat="1" ht="14.25"/>
-    <row r="389" s="30" customFormat="1" ht="14.25"/>
-    <row r="390" s="30" customFormat="1" ht="14.25"/>
-    <row r="391" s="30" customFormat="1" ht="14.25"/>
-    <row r="392" s="30" customFormat="1" ht="14.25"/>
-    <row r="393" s="30" customFormat="1" ht="14.25"/>
-    <row r="394" s="30" customFormat="1" ht="14.25"/>
-    <row r="395" s="30" customFormat="1" ht="14.25"/>
-    <row r="396" s="30" customFormat="1" ht="14.25"/>
-    <row r="397" s="30" customFormat="1" ht="14.25"/>
-    <row r="398" s="30" customFormat="1" ht="14.25"/>
-    <row r="399" s="30" customFormat="1" ht="14.25"/>
-    <row r="400" s="30" customFormat="1" ht="14.25"/>
-    <row r="401" s="30" customFormat="1" ht="14.25"/>
-    <row r="402" s="30" customFormat="1" ht="14.25"/>
-    <row r="403" s="30" customFormat="1" ht="14.25"/>
-    <row r="404" s="30" customFormat="1" ht="14.25"/>
-    <row r="405" s="30" customFormat="1" ht="14.25"/>
-    <row r="406" s="30" customFormat="1" ht="14.25"/>
-    <row r="407" s="30" customFormat="1" ht="14.25"/>
-    <row r="408" s="30" customFormat="1" ht="14.25"/>
-    <row r="409" s="30" customFormat="1" ht="14.25"/>
-    <row r="410" s="30" customFormat="1" ht="14.25"/>
-    <row r="411" s="30" customFormat="1" ht="14.25"/>
-    <row r="412" s="30" customFormat="1" ht="14.25"/>
-    <row r="413" s="30" customFormat="1" ht="14.25"/>
-    <row r="414" s="30" customFormat="1" ht="14.25"/>
-    <row r="415" s="30" customFormat="1" ht="14.25"/>
-    <row r="416" s="30" customFormat="1" ht="14.25"/>
-    <row r="417" s="30" customFormat="1" ht="14.25"/>
-    <row r="418" s="30" customFormat="1" ht="14.25"/>
-    <row r="419" s="30" customFormat="1" ht="14.25"/>
-    <row r="420" s="30" customFormat="1" ht="14.25"/>
-    <row r="421" s="30" customFormat="1" ht="14.25"/>
-    <row r="422" s="30" customFormat="1" ht="14.25"/>
-    <row r="423" s="30" customFormat="1" ht="14.25"/>
-    <row r="424" s="30" customFormat="1" ht="14.25"/>
-    <row r="425" s="30" customFormat="1" ht="14.25"/>
-    <row r="426" s="30" customFormat="1" ht="14.25"/>
-    <row r="427" s="30" customFormat="1" ht="14.25"/>
-    <row r="428" s="30" customFormat="1" ht="14.25"/>
-    <row r="429" s="30" customFormat="1" ht="14.25"/>
-    <row r="430" s="30" customFormat="1" ht="14.25"/>
-    <row r="431" s="30" customFormat="1" ht="14.25"/>
-    <row r="432" s="30" customFormat="1" ht="14.25"/>
-    <row r="433" s="30" customFormat="1" ht="14.25"/>
-    <row r="434" s="30" customFormat="1" ht="14.25"/>
-    <row r="435" s="30" customFormat="1" ht="14.25"/>
-    <row r="436" s="30" customFormat="1" ht="14.25"/>
-    <row r="437" s="30" customFormat="1" ht="14.25"/>
-    <row r="438" s="30" customFormat="1" ht="14.25"/>
-    <row r="439" s="30" customFormat="1" ht="14.25"/>
-    <row r="440" s="30" customFormat="1" ht="14.25"/>
-    <row r="441" s="30" customFormat="1" ht="14.25"/>
-    <row r="442" s="30" customFormat="1" ht="14.25"/>
-    <row r="443" s="30" customFormat="1" ht="14.25"/>
-    <row r="444" s="30" customFormat="1" ht="14.25"/>
-    <row r="445" s="30" customFormat="1" ht="14.25"/>
-    <row r="446" s="30" customFormat="1" ht="14.25"/>
-    <row r="447" s="30" customFormat="1" ht="14.25"/>
-    <row r="448" s="30" customFormat="1" ht="14.25"/>
-    <row r="449" s="30" customFormat="1" ht="14.25"/>
-    <row r="450" s="30" customFormat="1" ht="14.25"/>
-    <row r="451" s="30" customFormat="1" ht="14.25"/>
-    <row r="452" s="30" customFormat="1" ht="14.25"/>
-    <row r="453" s="30" customFormat="1" ht="14.25"/>
-    <row r="454" s="30" customFormat="1" ht="14.25"/>
-    <row r="455" s="30" customFormat="1" ht="14.25"/>
-    <row r="456" s="30" customFormat="1" ht="14.25"/>
-    <row r="457" s="30" customFormat="1" ht="14.25"/>
-    <row r="458" s="30" customFormat="1" ht="14.25"/>
-    <row r="459" s="30" customFormat="1" ht="14.25"/>
-    <row r="460" s="30" customFormat="1" ht="14.25"/>
-    <row r="461" s="30" customFormat="1" ht="14.25"/>
-    <row r="462" s="30" customFormat="1" ht="14.25"/>
-    <row r="463" s="30" customFormat="1" ht="14.25"/>
-    <row r="464" s="30" customFormat="1" ht="14.25"/>
-    <row r="465" s="30" customFormat="1" ht="14.25"/>
-    <row r="466" s="30" customFormat="1" ht="14.25"/>
-    <row r="467" s="30" customFormat="1" ht="14.25"/>
-    <row r="468" s="30" customFormat="1" ht="14.25"/>
-    <row r="469" s="30" customFormat="1" ht="14.25"/>
-    <row r="470" s="30" customFormat="1" ht="14.25"/>
-    <row r="471" s="30" customFormat="1" ht="14.25"/>
-    <row r="472" s="30" customFormat="1" ht="14.25"/>
-    <row r="473" s="30" customFormat="1" ht="14.25"/>
-    <row r="474" s="30" customFormat="1" ht="14.25"/>
-    <row r="475" s="30" customFormat="1" ht="14.25"/>
-    <row r="476" s="30" customFormat="1" ht="14.25"/>
-    <row r="477" s="30" customFormat="1" ht="14.25"/>
-    <row r="478" s="30" customFormat="1" ht="14.25"/>
-    <row r="479" s="30" customFormat="1" ht="14.25"/>
-    <row r="480" s="30" customFormat="1" ht="14.25"/>
-    <row r="481" s="30" customFormat="1" ht="14.25"/>
-    <row r="482" s="30" customFormat="1" ht="14.25"/>
-    <row r="483" s="30" customFormat="1" ht="14.25"/>
-    <row r="484" s="30" customFormat="1" ht="14.25"/>
-    <row r="485" s="30" customFormat="1" ht="14.25"/>
-    <row r="486" s="30" customFormat="1" ht="14.25"/>
-    <row r="487" s="30" customFormat="1" ht="14.25"/>
-    <row r="488" s="30" customFormat="1" ht="14.25"/>
-    <row r="489" s="30" customFormat="1" ht="14.25"/>
-    <row r="490" s="30" customFormat="1" ht="14.25"/>
-    <row r="491" s="30" customFormat="1" ht="14.25"/>
-    <row r="492" s="30" customFormat="1" ht="14.25"/>
-    <row r="493" s="30" customFormat="1" ht="14.25"/>
-    <row r="494" s="30" customFormat="1" ht="14.25"/>
-    <row r="495" s="30" customFormat="1" ht="14.25"/>
-    <row r="496" s="30" customFormat="1" ht="14.25"/>
-    <row r="497" s="30" customFormat="1" ht="14.25"/>
-    <row r="498" s="30" customFormat="1" ht="14.25"/>
-    <row r="499" s="30" customFormat="1" ht="14.25"/>
-    <row r="500" s="30" customFormat="1" ht="14.25"/>
-    <row r="501" s="30" customFormat="1" ht="14.25"/>
-    <row r="502" s="30" customFormat="1" ht="14.25"/>
-    <row r="503" s="30" customFormat="1" ht="14.25"/>
-    <row r="504" s="30" customFormat="1" ht="14.25"/>
-    <row r="505" s="30" customFormat="1" ht="14.25"/>
-    <row r="506" s="30" customFormat="1" ht="14.25"/>
-    <row r="507" s="30" customFormat="1" ht="14.25"/>
-    <row r="508" s="30" customFormat="1" ht="14.25"/>
-    <row r="509" s="30" customFormat="1" ht="14.25"/>
-    <row r="510" s="30" customFormat="1" ht="14.25"/>
-    <row r="511" s="30" customFormat="1" ht="14.25"/>
-    <row r="512" s="30" customFormat="1" ht="14.25"/>
-    <row r="513" s="30" customFormat="1" ht="14.25"/>
-    <row r="514" s="30" customFormat="1" ht="14.25"/>
-    <row r="515" s="30" customFormat="1" ht="14.25"/>
-    <row r="516" s="30" customFormat="1" ht="14.25"/>
-    <row r="517" s="30" customFormat="1" ht="14.25"/>
-    <row r="518" s="30" customFormat="1" ht="14.25"/>
-    <row r="519" s="30" customFormat="1" ht="14.25"/>
-    <row r="520" s="30" customFormat="1" ht="14.25"/>
-    <row r="521" s="30" customFormat="1" ht="14.25"/>
-    <row r="522" s="30" customFormat="1" ht="14.25"/>
-    <row r="523" s="30" customFormat="1" ht="14.25"/>
-    <row r="524" s="30" customFormat="1" ht="14.25"/>
-    <row r="525" s="30" customFormat="1" ht="14.25"/>
-    <row r="526" s="30" customFormat="1" ht="14.25"/>
-    <row r="527" s="30" customFormat="1" ht="14.25"/>
-    <row r="528" s="30" customFormat="1" ht="14.25"/>
-    <row r="529" s="30" customFormat="1" ht="14.25"/>
-    <row r="530" s="30" customFormat="1" ht="14.25"/>
-    <row r="531" s="30" customFormat="1" ht="14.25"/>
-    <row r="532" s="30" customFormat="1" ht="14.25"/>
-    <row r="533" s="30" customFormat="1" ht="14.25"/>
-    <row r="534" s="30" customFormat="1" ht="14.25"/>
-    <row r="535" s="30" customFormat="1" ht="14.25"/>
-    <row r="536" s="30" customFormat="1" ht="14.25"/>
-    <row r="537" s="30" customFormat="1" ht="14.25"/>
-    <row r="538" s="30" customFormat="1" ht="14.25"/>
-    <row r="539" s="30" customFormat="1" ht="14.25"/>
-    <row r="540" s="30" customFormat="1" ht="14.25"/>
-    <row r="541" s="30" customFormat="1" ht="14.25"/>
-    <row r="542" s="30" customFormat="1" ht="14.25"/>
-    <row r="543" s="30" customFormat="1" ht="14.25"/>
-    <row r="544" s="30" customFormat="1" ht="14.25"/>
-    <row r="545" s="30" customFormat="1" ht="14.25"/>
-    <row r="546" s="30" customFormat="1" ht="14.25"/>
-    <row r="547" s="30" customFormat="1" ht="14.25"/>
-    <row r="548" s="30" customFormat="1" ht="14.25"/>
-    <row r="549" s="30" customFormat="1" ht="14.25"/>
-    <row r="550" s="30" customFormat="1" ht="14.25"/>
-    <row r="551" s="30" customFormat="1" ht="14.25"/>
-    <row r="552" s="30" customFormat="1" ht="14.25"/>
-    <row r="553" s="30" customFormat="1" ht="14.25"/>
-    <row r="554" s="30" customFormat="1" ht="14.25"/>
-    <row r="555" s="30" customFormat="1" ht="14.25"/>
-    <row r="556" s="30" customFormat="1" ht="14.25"/>
-    <row r="557" s="30" customFormat="1" ht="14.25"/>
-    <row r="558" s="30" customFormat="1" ht="14.25"/>
-    <row r="559" s="30" customFormat="1" ht="14.25"/>
-    <row r="560" s="30" customFormat="1" ht="14.25"/>
-    <row r="561" s="30" customFormat="1" ht="14.25"/>
-    <row r="562" s="30" customFormat="1" ht="14.25"/>
-    <row r="563" s="30" customFormat="1" ht="14.25"/>
-    <row r="564" s="30" customFormat="1" ht="14.25"/>
-    <row r="565" s="30" customFormat="1" ht="14.25"/>
-    <row r="566" s="30" customFormat="1" ht="14.25"/>
-    <row r="567" s="30" customFormat="1" ht="14.25"/>
-    <row r="568" s="30" customFormat="1" ht="14.25"/>
-    <row r="569" s="30" customFormat="1" ht="14.25"/>
-    <row r="570" s="30" customFormat="1" ht="14.25"/>
-    <row r="571" s="30" customFormat="1" ht="14.25"/>
-    <row r="572" s="30" customFormat="1" ht="14.25"/>
-    <row r="573" s="30" customFormat="1" ht="14.25"/>
-    <row r="574" s="30" customFormat="1" ht="14.25"/>
-    <row r="575" s="30" customFormat="1" ht="14.25"/>
-    <row r="576" s="30" customFormat="1" ht="14.25"/>
-    <row r="577" s="30" customFormat="1" ht="14.25"/>
-    <row r="578" s="30" customFormat="1" ht="14.25"/>
-    <row r="579" s="30" customFormat="1" ht="14.25"/>
-    <row r="580" s="30" customFormat="1" ht="14.25"/>
-    <row r="581" s="30" customFormat="1" ht="14.25"/>
-    <row r="582" s="30" customFormat="1" ht="14.25"/>
-    <row r="583" s="30" customFormat="1" ht="14.25"/>
-    <row r="584" s="30" customFormat="1" ht="14.25"/>
-    <row r="585" s="30" customFormat="1" ht="14.25"/>
-    <row r="586" s="30" customFormat="1" ht="14.25"/>
-    <row r="587" s="30" customFormat="1" ht="14.25"/>
-    <row r="588" s="30" customFormat="1" ht="14.25"/>
-    <row r="589" s="30" customFormat="1" ht="14.25"/>
-    <row r="590" s="30" customFormat="1" ht="14.25"/>
-    <row r="591" s="30" customFormat="1" ht="14.25"/>
-    <row r="592" s="30" customFormat="1" ht="14.25"/>
-    <row r="593" s="30" customFormat="1" ht="14.25"/>
-    <row r="594" s="30" customFormat="1" ht="14.25"/>
-    <row r="595" s="30" customFormat="1" ht="14.25"/>
-    <row r="596" s="30" customFormat="1" ht="14.25"/>
-    <row r="597" s="30" customFormat="1" ht="14.25"/>
-    <row r="598" s="30" customFormat="1" ht="14.25"/>
-    <row r="599" s="30" customFormat="1" ht="14.25"/>
-    <row r="600" s="30" customFormat="1" ht="14.25"/>
-    <row r="601" s="30" customFormat="1" ht="14.25"/>
-    <row r="602" s="30" customFormat="1" ht="14.25"/>
-    <row r="603" s="30" customFormat="1" ht="14.25"/>
-    <row r="604" s="30" customFormat="1" ht="14.25"/>
-    <row r="605" s="30" customFormat="1" ht="14.25"/>
-    <row r="606" s="30" customFormat="1" ht="14.25"/>
-    <row r="607" s="30" customFormat="1" ht="14.25"/>
-    <row r="608" s="30" customFormat="1" ht="14.25"/>
-    <row r="609" s="30" customFormat="1" ht="14.25"/>
-    <row r="610" s="30" customFormat="1" ht="14.25"/>
+    <row r="237" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="238" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="239" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="240" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="241" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="242" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="243" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="244" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="245" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="246" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="247" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="248" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="249" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="250" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="251" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="252" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="253" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="254" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="255" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="256" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="257" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="258" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="259" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="260" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="261" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="262" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="263" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="264" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="265" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="266" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="267" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="268" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="269" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="270" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="271" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="272" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="273" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="274" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="275" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="276" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="277" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="278" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="279" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="280" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="281" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="282" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="283" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="284" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="285" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="286" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="287" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="288" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="289" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="290" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="291" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="292" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="293" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="294" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="295" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="296" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="297" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="298" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="299" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="300" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="301" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B301" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="302" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="C302" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="303" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="304" spans="2:3" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B304" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="305" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="306" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B306" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="307" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="308" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B308" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="309" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="310" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="311" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="312" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="313" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="314" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="315" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="316" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="317" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="318" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="319" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="320" spans="2:2" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="321" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="322" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="323" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="324" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="325" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="326" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="327" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="328" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="329" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="330" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="331" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="332" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="333" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="334" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="335" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="336" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="337" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="338" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="339" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="340" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="341" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="342" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="343" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="344" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="345" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="346" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="347" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="348" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="349" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="350" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="351" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="352" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="353" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="354" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="355" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="356" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="357" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="358" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="359" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="360" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="361" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="362" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="363" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="364" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="365" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="366" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="367" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="368" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="369" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="370" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="371" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="372" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="373" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="374" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="375" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="376" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="377" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="378" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="379" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="380" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="381" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="382" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="383" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="384" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="385" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="386" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="387" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="388" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="389" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="390" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="391" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="392" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="393" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="394" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="395" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="396" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="397" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="398" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="399" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="400" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="401" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="402" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="403" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="404" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="405" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="406" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="407" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="408" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="409" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="410" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="411" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="412" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="413" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="414" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="415" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="416" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="417" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="418" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="419" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="420" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="421" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="422" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="423" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="424" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="425" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="426" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="427" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="428" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="429" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="430" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="431" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="432" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="433" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="434" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="435" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="436" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="437" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="438" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="439" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="440" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="441" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="442" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="443" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="444" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="445" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="446" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="447" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="448" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="449" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="450" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="451" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="452" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="453" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="454" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="455" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="456" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="457" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="458" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="459" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="460" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="461" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="462" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="463" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="464" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="465" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="466" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="467" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="468" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="469" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="470" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="471" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="472" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="473" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="474" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="475" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="476" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="477" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="478" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="479" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="480" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="481" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="482" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="483" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="484" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="485" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="486" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="487" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="488" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="489" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="490" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="491" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="492" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="493" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="494" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="495" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="496" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="497" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="498" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="499" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="500" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="501" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="502" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="503" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="504" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="505" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="506" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="507" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="508" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="509" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="510" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="511" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="512" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="513" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="514" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="515" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="516" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="517" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="518" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="519" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="520" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="521" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="522" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="523" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="524" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="525" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="526" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="527" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="528" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="529" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="530" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="531" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="532" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="533" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="534" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="535" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="536" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="537" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="538" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="539" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="540" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="541" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="542" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="543" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="544" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="545" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="546" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="547" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="548" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="549" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="550" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="551" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="552" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="553" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="554" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="555" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="556" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="557" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="558" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="559" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="560" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="561" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="562" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="563" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="564" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="565" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="566" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="567" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="568" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="569" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="570" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="571" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="572" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="573" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="574" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="575" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="576" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="577" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="578" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="579" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="580" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="581" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="582" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="583" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="584" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="585" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="586" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="587" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="588" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="589" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="590" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="591" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="592" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="593" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="594" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="595" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="596" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="597" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="598" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="599" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="600" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="601" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="602" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="603" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="604" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="605" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="606" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="607" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="608" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="609" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="610" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="611" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="612" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="613" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="614" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="615" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="616" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="617" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="618" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="619" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="620" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="621" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="622" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="623" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="624" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="625" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="626" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="627" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="628" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="629" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="630" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="631" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="632" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="633" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
+    <row r="634" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3269,16 +3760,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:15" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="O1" location="目录!A1" display="返回"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" ht="18.75">
+    <row r="1" spans="1:15" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>22</v>
       </c>
@@ -3296,17 +3820,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" ht="18.75">
+    <row r="1" spans="1:15" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>22</v>
       </c>
@@ -3321,5 +3845,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>